<commit_message>
changes on manu's other computer
</commit_message>
<xml_diff>
--- a/data/haver_names.xlsx
+++ b/data/haver_names.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scampbell\Documents\GitHub\fim\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malcalakovalski\Documents\fim\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FA5AAF2-2A80-4FCA-AF26-A589BCA44FAB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D110C14-8E2C-4DB3-B8E3-E9CCECF06202}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="75" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="131">
   <si>
     <t>code</t>
   </si>
@@ -408,7 +408,19 @@
     <t>gross_consumption_grants</t>
   </si>
   <si>
-    <t>(consumption grants + medicaid grants, or all grants in aid to s+l (not igrants))</t>
+    <t>snap</t>
+  </si>
+  <si>
+    <t>yptol</t>
+  </si>
+  <si>
+    <t>wages_lost_assistance</t>
+  </si>
+  <si>
+    <t>gftffx</t>
+  </si>
+  <si>
+    <t>date</t>
   </si>
 </sst>
 </file>
@@ -452,9 +464,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -795,10 +810,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C64"/>
+  <dimension ref="A1:B67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="96" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" zoomScale="96" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -814,519 +829,550 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
+    <row r="2" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>80</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>16</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>18</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>19</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>20</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>21</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
         <v>22</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>24</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
         <v>25</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>26</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>27</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
         <v>28</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
         <v>29</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
         <v>30</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
         <v>31</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
         <v>32</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
         <v>33</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>105</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>34</v>
-      </c>
-      <c r="B32" t="s">
-        <v>125</v>
-      </c>
-      <c r="C32" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B33" t="s">
-        <v>107</v>
+        <v>125</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B35" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B36" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B37" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B38" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B39" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B40" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B41" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B42" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B43" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B44" t="s">
-        <v>47</v>
+        <v>115</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B45" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>118</v>
+        <v>48</v>
       </c>
       <c r="B46" t="s">
-        <v>119</v>
+        <v>49</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>50</v>
+        <v>118</v>
       </c>
       <c r="B47" t="s">
-        <v>71</v>
+        <v>119</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B48" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B49" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B50" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B51" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="B52" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B53" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>116</v>
+        <v>67</v>
       </c>
       <c r="B54" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>55</v>
+        <v>116</v>
       </c>
       <c r="B55" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>117</v>
+        <v>78</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>62</v>
+        <v>117</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B60" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>120</v>
+        <v>65</v>
       </c>
       <c r="B63" t="s">
-        <v>121</v>
+        <v>66</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
+        <v>120</v>
+      </c>
+      <c r="B64" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>127</v>
+      </c>
+      <c r="B65" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
         <v>122</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B66" t="s">
         <v>123</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>129</v>
+      </c>
+      <c r="B67" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FA9F3DB0CD4D844B918872BCED9B9CF9" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="61f75d9b13a46a58fd2456a565edcb9c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cac5d118-ba7b-4807-b700-df6f95cfff50" xmlns:ns3="66951ee6-cd93-49c7-9437-e871b2a117d6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d86870d415110e2c98f3a885b29630d1" ns2:_="" ns3:_="">
     <xsd:import namespace="cac5d118-ba7b-4807-b700-df6f95cfff50"/>
@@ -1543,15 +1589,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1559,6 +1596,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11C50A7A-072C-42B0-A807-112C623C860C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6FBE834-A7AF-4CA7-B4B3-E5BBA0B171E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1573,14 +1618,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11C50A7A-072C-42B0-A807-112C623C860C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
haver data pull 6/24/21
</commit_message>
<xml_diff>
--- a/data/haver_names.xlsx
+++ b/data/haver_names.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malcalakovalski\Documents\fim\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scampbell\Documents\GitHub\fim\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D110C14-8E2C-4DB3-B8E3-E9CCECF06202}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EEC58FC-327E-4FDC-BE43-B694FE08AA6B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="75" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="130">
   <si>
     <t>code</t>
   </si>
@@ -418,9 +418,6 @@
   </si>
   <si>
     <t>gftffx</t>
-  </si>
-  <si>
-    <t>date</t>
   </si>
 </sst>
 </file>
@@ -464,12 +461,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -810,10 +804,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B67"/>
+  <dimension ref="A1:B66"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -829,531 +823,523 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>130</v>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>92</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>96</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B24" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B25" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B31" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B32" t="s">
-        <v>105</v>
+        <v>125</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B34" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B35" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B36" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B37" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B38" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B39" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B40" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B41" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B42" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B43" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B44" t="s">
-        <v>115</v>
+        <v>47</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B45" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>48</v>
+        <v>118</v>
       </c>
       <c r="B46" t="s">
-        <v>49</v>
+        <v>119</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>118</v>
+        <v>50</v>
       </c>
       <c r="B47" t="s">
-        <v>119</v>
+        <v>71</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B48" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B49" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B50" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B51" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="B52" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B53" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>67</v>
+        <v>116</v>
       </c>
       <c r="B54" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>116</v>
+        <v>55</v>
       </c>
       <c r="B55" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B56" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B57" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B58" t="s">
-        <v>78</v>
+        <v>117</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B59" t="s">
-        <v>117</v>
+        <v>62</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B62" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>65</v>
+        <v>120</v>
       </c>
       <c r="B63" t="s">
-        <v>66</v>
+        <v>121</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B64" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B65" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="B66" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A67" t="s">
-        <v>129</v>
-      </c>
-      <c r="B67" t="s">
         <v>126</v>
       </c>
     </row>
@@ -1373,6 +1359,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FA9F3DB0CD4D844B918872BCED9B9CF9" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="61f75d9b13a46a58fd2456a565edcb9c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cac5d118-ba7b-4807-b700-df6f95cfff50" xmlns:ns3="66951ee6-cd93-49c7-9437-e871b2a117d6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d86870d415110e2c98f3a885b29630d1" ns2:_="" ns3:_="">
     <xsd:import namespace="cac5d118-ba7b-4807-b700-df6f95cfff50"/>
@@ -1589,12 +1581,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11C50A7A-072C-42B0-A807-112C623C860C}">
   <ds:schemaRefs>
@@ -1604,6 +1590,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C7CC3BF-DF9F-4E15-B3E2-3F2BE52E9D01}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="66951ee6-cd93-49c7-9437-e871b2a117d6"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="cac5d118-ba7b-4807-b700-df6f95cfff50"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6FBE834-A7AF-4CA7-B4B3-E5BBA0B171E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1620,21 +1623,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C7CC3BF-DF9F-4E15-B3E2-3F2BE52E9D01}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="cac5d118-ba7b-4807-b700-df6f95cfff50"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="66951ee6-cd93-49c7-9437-e871b2a117d6"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
haver pull with social security
gftfbdx was missing in haver pivoted
</commit_message>
<xml_diff>
--- a/data/haver_names.xlsx
+++ b/data/haver_names.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scampbell\Documents\GitHub\fim\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malcalakovalski\Documents\fim\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25310A0F-BA5E-4259-B62D-F054092E9F8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DF3DC16-585A-427E-9D83-5EAFCF8B9A4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6020" yWindow="1870" windowWidth="9600" windowHeight="4910" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="146">
   <si>
     <t>code</t>
   </si>
@@ -460,6 +460,12 @@
   </si>
   <si>
     <t>yri</t>
+  </si>
+  <si>
+    <t>gftfbdx</t>
+  </si>
+  <si>
+    <t>social_security</t>
   </si>
 </sst>
 </file>
@@ -846,10 +852,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B73"/>
+  <dimension ref="A1:B74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="96" workbookViewId="0">
-      <selection activeCell="A70" sqref="A70"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="96" workbookViewId="0">
+      <selection activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1441,6 +1447,14 @@
         <v>142</v>
       </c>
     </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>144</v>
+      </c>
+      <c r="B74" t="s">
+        <v>145</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -1448,18 +1462,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1680,6 +1694,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11C50A7A-072C-42B0-A807-112C623C860C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C7CC3BF-DF9F-4E15-B3E2-3F2BE52E9D01}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -1692,14 +1714,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="cac5d118-ba7b-4807-b700-df6f95cfff50"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11C50A7A-072C-42B0-A807-112C623C860C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>